<commit_message>
Major update: Sub-packs, tabular UI, tricky word review, and progressive difficulty
Features Added:
- Sub-pack organization: 3 sub-packs (Year 1 High Frequency, Short Vowels, Consonant Blends)
- Tabular UI: Sortable pack table with columns for Pack #, Title, Words, Last Reviewed, Progress
- Tricky word review at 3 levels: Global, Sub-pack, Pack
- Last Reviewed tracking: Shows when packs were fully completed
- Progressive difficulty ordering: Packs reordered from easiest to hardest
- 20 packs deployed (testing before scaling to 130)

Technical Changes:
- Complete rewrite of app.js with new features
- Updated index.html for tabular layout
- Enhanced style.css with table styles, sub-pack sections
- Excel synced to show current 20 packs
- Added extract_all_packs.py and reorganize_by_difficulty.py scripts

Total words: 547 across 20 packs
Total unique sub-packs: 3

Next step: Test thoroughly, then expand to all 130 packs
</commit_message>
<xml_diff>
--- a/Phonics_Word_Bank.xlsx
+++ b/Phonics_Word_Bank.xlsx
@@ -542,272 +542,272 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>P5: 0B. YEAR 2 COMMON EXCEPTION - Pack 1</t>
+          <t>P5: 1. SHORT VOWEL A - Pack 1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>64 statutory words for Year 2 (Pack 1 of 3)</t>
+          <t>CVC words with 'a' as in cat (Pack 1 of 2)</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>after, again, any, bath, beautiful, because, behind, both, break, busy, child, children, christmas, class, climb, clothes, cold, could, door, even, every, everybody, eye, fast, father, find, floor, gold, grass, great</t>
+          <t>assistant, attack, attic, bad, bag, bat, cab, cap, cat, dab, fan, fat, gal, gap, gas, ham, has, hat, jab, jam, kit, lap, mad, man, map, mat, max, nag, nap, napkin</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>P6: 0B. YEAR 2 COMMON EXCEPTION - Pack 2</t>
+          <t>P6: 1. SHORT VOWEL A - Pack 2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>64 statutory words for Year 2 (Pack 2 of 3)</t>
+          <t>CVC words with 'a' as in cat (Pack 2 of 2)</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>half, hold, hour, improve, kind, last, many, mind, money, most, move, mr, mrs, old, only, parents, pass, past, path, people, plant, poor, pretty, prove, should, steak, sugar, sure, told, water</t>
+          <t>pal, pan, pasta, pat, rag, ram, ran, rap, rat, sad, sap, sat, span, spank, spick, stack, tab, tact, tag, tan, tap, tax, van, wag, wax, yam, zap</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>P7: 0B. YEAR 2 COMMON EXCEPTION - Pack 3</t>
+          <t>P7: 1. SHORT VOWEL E - Pack 1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>64 statutory words for Year 2 (Pack 3 of 3)</t>
+          <t>CVC words with 'e' as in bed (Pack 1 of 2)</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>who, whole, wild, would</t>
+          <t>antenna, antiseptic, arrest, bed, beg, bell, ben, best, bet, cassette, deck, den, fed, fell, gem, hem, hen, insect, inspect, jet, kitten, led, leg, less, let, men, mess, met, neck, nest</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>P8: 0C. YEAR 3/4 COMMON EXCEPTION - Pack 1</t>
+          <t>P8: 1. SHORT VOWEL E - Pack 2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>100 statutory words for Years 3 &amp; 4 (Pack 1 of 4)</t>
+          <t>CVC words with 'e' as in bed (Pack 2 of 2)</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>accident, accidentally, actual, actually, address, although, answer, appear, arrive, believe, bicycle, breath, breathe, build, business, busy, calendar, caught, centre, century, certain, circle, complete, consider, continue, decide, describe, different, difficult, disappear</t>
+          <t>net, packet, peck, peg, pen, pest, pet, red, rest, sell, sense, sent, set, speck, step, tell, ten, tennis, tense, tent, test, ticket, vest, vet, wed, well, west, wet, yell, yet</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>P9: 0C. YEAR 3/4 COMMON EXCEPTION - Pack 2</t>
+          <t>P9: 1. SHORT VOWEL I - Pack 1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>100 statutory words for Years 3 &amp; 4 (Pack 2 of 4)</t>
+          <t>CVC words with 'i' as in sit (Pack 1 of 2)</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>early, earth, eight, eighth, enough, exercise, experience, experiment, extreme, famous, favourite, february, forward, forwards, fruit, grammar, group, guard, guide, heard, heart, height, history, imagine, important, increase, interest, island, knowledge, learn</t>
+          <t>ant, assist, bib, bin, bit, did, dig, dim, din, dip, fig, fin, fit, fix, gig, hid, hip, hit, insist, its, jig, kick, kid, lick, lid, lip, lit, mix, nip, nit</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>P10: 0C. YEAR 3/4 COMMON EXCEPTION - Pack 3</t>
+          <t>P10: 1. SHORT VOWEL I - Pack 2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>100 statutory words for Years 3 &amp; 4 (Pack 3 of 4)</t>
+          <t>CVC words with 'i' as in sit (Pack 2 of 2)</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>length, library, material, medicine, mention, minute, natural, naughty, notice, occasion, occasionally, often, opposite, ordinary, particular, peculiar, perhaps, popular, position, possess, possession, possible, potatoes, pressure, probably, promise, purpose, quarter, question, recent</t>
+          <t>pant, pants, pick, pig, pin, pip, pit, rib, rid, rig, rim, rip, sick, sip, sit, six, snap, snip, spat, spin, spit, tick, tin, tip, wick, wig, win, wit, zip</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>P11: 0C. YEAR 3/4 COMMON EXCEPTION - Pack 4</t>
+          <t>P11: 1. SHORT VOWEL O - Pack 1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>100 statutory words for Years 3 &amp; 4 (Pack 4 of 4)</t>
+          <t>CVC words with 'o' as in dog (Pack 1 of 3)</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>regular, reign, remember, sentence, separate, special, straight, strange, strength, suppose, surprise, therefore, though, thought, through, various, weight</t>
+          <t>across, adopt, block, bob, bog, box, cannon, cannot, carrot, clock, cob, cod, cog, comic, connect, correct, cost, cot, cotton, crop, cross, desktop, dock, dog, dot, dragon, drop, fog, fox, god</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>P12: 0D. YEAR 5/6 STATUTORY SPELLING - Pack 1</t>
+          <t>P12: 1. SHORT VOWEL O - Pack 2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>100 statutory spelling words for Years 5 &amp; 6 (Pack 1 of 4)</t>
+          <t>CVC words with 'o' as in dog (Pack 2 of 3)</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>accommodate, accompany, according, achieve, aggressive, amateur, ancient, apparent, appreciate, attached, available, average, awkward, bargain, bruise, category, cemetery, committee, communicate, community, competition, conscience, conscious, controversy, convenience, correspond, criticise, curiosity, definite, desperate</t>
+          <t>haddock, hog, hop, hot, incorrect, job, jog, jot, kiosk, lock, log, lot, maggot, mob, mock, mom, mop, moss, nod, nonsense, odd, opinion, parrot, pocket, pod, pond, pop, pot, pox, protect</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>P13: 0D. YEAR 5/6 STATUTORY SPELLING - Pack 2</t>
+          <t>P13: 1. SHORT VOWEL O - Pack 3</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>100 statutory spelling words for Years 5 &amp; 6 (Pack 2 of 4)</t>
+          <t>CVC words with 'o' as in dog (Pack 3 of 3)</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>determined, develop, dictionary, disastrous, embarrass, environment, equip, equipment, especially, exaggerate, excellent, existence, explanation, familiar, foreign, forty, frequently, government, guarantee, harass, hindrance, identity, immediate, immediately, individual, interfere, interrupt, language, leisure, lightning</t>
+          <t>reckon, rob, rock, rocket, rod, rot, second, shock, sob, sock, spot, spotted, stop, ticktock, top, topic, trod, trot</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>P14: 0D. YEAR 5/6 STATUTORY SPELLING - Pack 3</t>
+          <t>P14: 1. SHORT VOWEL U - Pack 1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>100 statutory spelling words for Years 5 &amp; 6 (Pack 3 of 4)</t>
+          <t>CVC words with 'u' as in cup (Pack 1 of 3)</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>marvellous, mischievous, muscle, necessary, neighbour, nuisance, occupy, occur, opportunity, parliament, persuade, physical, prejudice, privilege, profession, programme, pronunciation, queue, recognise, recommend, relevant, restaurant, rhyme, rhythm, sacrifice, secretary, shoulder, signature, sincere, sincerely</t>
+          <t>bud, bug, bump, bun, bus, crust, cub, cud, cup, cut, discuss, drug, drum, drunk, duck, dug, dumb, dump, dust, eggcup, fun, grunt, gum, gun, gust, gut, hiccup, hippopotamus, hug, hum</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>P15: 0D. YEAR 5/6 STATUTORY SPELLING - Pack 4</t>
+          <t>P15: 1. SHORT VOWEL U - Pack 2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>100 statutory spelling words for Years 5 &amp; 6 (Pack 4 of 4)</t>
+          <t>CVC words with 'u' as in cup (Pack 2 of 3)</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>soldier, stomach, sufficient, suggest, symbol, system, temperature, thorough, twelfth, variety, vegetable, vehicle, yacht</t>
+          <t>hump, hunt, hut, instruct, jug, jump, jut, lump, minimum, mud, mug, mumps, must, nun, nut, product, pub, pump, pumpkin, pun, pup, puppet, putt, rub, rucksack, rug, rump, run, rust, rut</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>P16: 1. SHORT VOWEL A - Pack 1</t>
+          <t>P16: 1. SHORT VOWEL U - Pack 3</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CVC words with 'a' as in cat (Pack 1 of 2)</t>
+          <t>CVC words with 'u' as in cup (Pack 3 of 3)</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>assistant, attack, attic, bad, bag, bat, cab, cap, cat, dab, fan, fat, gal, gap, gas, ham, has, hat, jab, jam, kit, lap, mad, man, map, mat, max, nag, nap, napkin</t>
+          <t>scrub, skunk, snug, spun, stuck, stump, sub, suck, sudden, sum, sun, sunk, sunset, suntan, tantrum, truck, trumpet, trunk, trust, tub, tuck, tug, tusk, undid, undress, unpack, upon, upset, us, yum</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>P17: 1. SHORT VOWEL A - Pack 2</t>
+          <t>P17: 2. 3-LETTER BLENDS</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CVC words with 'a' as in cat (Pack 2 of 2)</t>
+          <t>scr, spr, str, spl, thr</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>pal, pan, pasta, pat, rag, ram, ran, rap, rat, sad, sap, sat, span, spank, spick, stack, tab, tact, tag, tan, tap, tax, van, wag, wax, yam, zap</t>
+          <t>scrape, screen, screw, splash, splendid, splint, sprain, spray, spread, spring, sprout, strap, stream, street, string, strip, strong, three, throat, throne, throw</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>P18: 1. SHORT VOWEL E - Pack 1</t>
+          <t>P18: 2. L-BLENDS - Pack 1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CVC words with 'e' as in bed (Pack 1 of 2)</t>
+          <t>bl, cl, fl, gl, pl, sl (Pack 1 of 2)</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>antenna, antiseptic, arrest, bed, beg, bell, ben, best, bet, cassette, deck, den, fed, fell, gem, hem, hen, insect, inspect, jet, kitten, led, leg, less, let, men, mess, met, neck, nest</t>
+          <t>black, blast, blend, bless, blob, blot, blue, blunt, clamp, clap, clip, club, clump, flag, flan, flat, flip, flock, flop, flow, glad, glass, glide, glow, glue, glum, plan, plank, play, plot</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>P19: 1. SHORT VOWEL E - Pack 2</t>
+          <t>P19: 2. L-BLENDS - Pack 2</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CVC words with 'e' as in bed (Pack 2 of 2)</t>
+          <t>bl, cl, fl, gl, pl, sl (Pack 2 of 2)</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>net, packet, peck, peg, pen, pest, pet, red, rest, sell, sense, sent, set, speck, step, tell, ten, tennis, tense, tent, test, ticket, vest, vet, wed, well, west, wet, yell, yet</t>
+          <t>plug, plum, plump, plus, skill, skull, slam, slap, sled, slept, slid, slim, slip, slit, slot, slow, slug, smell, spell, spelt, spill, split</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>P20: 1. SHORT VOWEL I - Pack 1</t>
+          <t>P20: 2. R-BLENDS - Pack 1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CVC words with 'i' as in sit (Pack 1 of 2)</t>
+          <t>br, cr, dr, fr, gr, pr, tr (Pack 1 of 2)</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>ant, assist, bib, bin, bit, did, dig, dim, din, dip, fig, fin, fit, fix, gig, hid, hip, hit, insist, its, jig, kick, kid, lick, lid, lip, lit, mix, nip, nit</t>
+          <t>brave, brick, bring, brown, brush, crab, crack, crash, crown, cry, drab, drag, dress, drill, drip, frank, frantic, free, fresh, frill, frog, frost, grab, gram, green, grim, grin, grip, pray, press</t>
         </is>
       </c>
     </row>

</xml_diff>